<commit_message>
Sprint-1 Project Backlog is done
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Text Transformer</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t>Task #3 Implement CapitalizeTransformer class.</t>
+  </si>
+  <si>
+    <t>Task #1 Implement InverseTransformer class with logic to preserve case positions.</t>
+  </si>
+  <si>
+    <t>Task #2 Write unit tests for edge cases (e.g., single character, empty string, mixed case).</t>
+  </si>
+  <si>
+    <t>Task #1 Implement LatexTransformer class to handle &amp; and $.</t>
+  </si>
+  <si>
+    <t>Task #1 Implement RemoveRepetitiveWordsTransformer class using regular expressions or a loop.</t>
+  </si>
+  <si>
+    <t>Task #2 Test with multiple repetitions</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1278,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.8" outlineLevelCol="4"/>
@@ -1426,10 +1441,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.8" outlineLevelCol="2"/>
@@ -1502,6 +1517,55 @@
         <v>35</v>
       </c>
     </row>
+    <row r="17" ht="45" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:2">
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="2:2">
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" ht="45" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="2:2">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" ht="45" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" ht="30" spans="2:2">
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="2:2">
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>